<commit_message>
updated with remaining components
</commit_message>
<xml_diff>
--- a/BOM/BOM KeyBoard.xlsx
+++ b/BOM/BOM KeyBoard.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22624"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22730"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\projects\upl_audioanalyzer\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E2EBB78-9430-4DFB-8A3E-72DDA3A14A3A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F971166-DCD6-48D5-94A9-4E070AA7E3C9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="6555" yWindow="2940" windowWidth="21600" windowHeight="11385" xr2:uid="{3C56C210-DCD0-4B76-B854-73BBFDBB2958}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3C56C210-DCD0-4B76-B854-73BBFDBB2958}"/>
   </bookViews>
   <sheets>
     <sheet name="FetHead" sheetId="3" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="18">
   <si>
     <t>Farnell</t>
   </si>
@@ -75,10 +75,16 @@
     <t>Button</t>
   </si>
   <si>
-    <t>Hartin Connector</t>
-  </si>
-  <si>
     <t>LED 1206</t>
+  </si>
+  <si>
+    <t>Hartin Connector Chassis</t>
+  </si>
+  <si>
+    <t>Hartin Connector Cable</t>
+  </si>
+  <si>
+    <t>25-26 ribbon cable.</t>
   </si>
 </sst>
 </file>
@@ -449,17 +455,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B339EA2E-58E6-48C2-B743-24C662D28A88}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.42578125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.140625" customWidth="1"/>
-    <col min="6" max="6" width="21" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="23.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.25">
@@ -492,12 +498,9 @@
       <c r="C2">
         <v>1</v>
       </c>
-      <c r="D2">
-        <v>0.13</v>
-      </c>
       <c r="E2">
-        <f t="shared" ref="E2:E9" si="0">C2*D2</f>
-        <v>0.13</v>
+        <f t="shared" ref="E2:E7" si="0">C2*D2</f>
+        <v>0</v>
       </c>
       <c r="F2" t="s">
         <v>3</v>
@@ -542,55 +545,89 @@
         <v>2.84</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>1106731</v>
+      </c>
       <c r="B5" t="s">
         <v>0</v>
       </c>
       <c r="C5">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="D5">
-        <v>0.05</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="E5">
         <f t="shared" si="0"/>
-        <v>0.30000000000000004</v>
+        <v>2.5499999999999998</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="2"/>
+      <c r="A6" s="1"/>
+      <c r="B6" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="1"/>
+      <c r="B7" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>0.05</v>
+      </c>
+      <c r="E7">
+        <f t="shared" si="0"/>
+        <v>0.30000000000000004</v>
+      </c>
+      <c r="F7" t="s">
+        <v>14</v>
+      </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A8" s="3"/>
+      <c r="A8" s="2"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9" s="1"/>
     </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="3"/>
+    </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="D11" t="s">
+      <c r="A11" s="1"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="D13" t="s">
         <v>11</v>
       </c>
-      <c r="E11">
-        <f>SUM(E2:E9)</f>
-        <v>40.120000000000005</v>
+      <c r="E13">
+        <f>SUM(E2:E11)</f>
+        <v>42.539999999999992</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="A3" r:id="rId1" display="760-3126" xr:uid="{8FF02029-F92B-4D12-94A4-629EE4CECCE6}"/>
     <hyperlink ref="A4" r:id="rId2" display="https://be.farnell.com/harting/09-18-526-7914/header-straight-s-latch-26way/dp/1106765" xr:uid="{F0419CBF-5412-41F1-8D23-F424748E6763}"/>
+    <hyperlink ref="A5" r:id="rId3" display="1106731" xr:uid="{B95F766E-EE43-4D7F-9AF1-D5C5AD2277A1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId4"/>
 </worksheet>
 </file>
</xml_diff>